<commit_message>
update bank_parser_py dependency URL, and enhance main.py with new data structures and transaction comparison logic
</commit_message>
<xml_diff>
--- a/conciliacion.xlsx
+++ b/conciliacion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOVIEMBRE" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,110 +17,109 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="11">
     <font>
       <name val="Aptos Narrow"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
-      <color indexed="12"/>
+      <color rgb="FF0000FF"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
-      <color indexed="12"/>
+      <color rgb="FF0000FF"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="1"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color indexed="12"/>
+      <color rgb="FF0000FF"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color indexed="12"/>
+      <color rgb="FF0000FF"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
       <family val="2"/>
-      <b val="1"/>
-      <color indexed="10"/>
+      <color rgb="FF000000"/>
       <sz val="8"/>
     </font>
     <font>
       <name val="Aptos Narrow"/>
+      <charset val="1"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="8"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="8"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="8"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,18 +132,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -153,7 +141,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -162,193 +150,141 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="3">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="17" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="15" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Comma 2" xfId="4"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Comma 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="4"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF7030A0"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
       <rgbColor rgb="00003366"/>
       <rgbColor rgb="00339966"/>
       <rgbColor rgb="00003300"/>
@@ -363,7 +299,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -686,16 +622,16 @@
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.33203125" defaultRowHeight="14.25"/>
   <cols>
-    <col width="7.5703125" customWidth="1" min="4" max="4"/>
-    <col width="12.42578125" customWidth="1" min="5" max="5"/>
-    <col width="13.85546875" customWidth="1" min="8" max="8"/>
-    <col width="12.42578125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="7.53125" customWidth="1" min="4" max="4"/>
+    <col width="12.33203125" customWidth="1" min="5" max="5"/>
+    <col width="13.796875" customWidth="1" min="8" max="8"/>
+    <col width="12.33203125" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -705,13 +641,13 @@
           <t>EMPRESA</t>
         </is>
       </c>
-      <c r="C1" s="54" t="inlineStr">
-        <is>
-          <t>EVOLUCION MULTIMEDIA MEXICO S DE RL DE CV</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="n"/>
-      <c r="E1" s="4" t="n"/>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>LA MISION</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="n"/>
+      <c r="E1" s="5" t="n"/>
       <c r="F1" s="2" t="n"/>
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="n"/>
@@ -727,13 +663,13 @@
           <t>MES</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>FEBRERO 2025</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="4" t="n"/>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>JUNIO 2025</t>
+        </is>
+      </c>
+      <c r="D2" s="7" t="n"/>
+      <c r="E2" s="5" t="n"/>
       <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
@@ -749,13 +685,13 @@
           <t>CUENTA</t>
         </is>
       </c>
-      <c r="C3" s="55" t="inlineStr">
-        <is>
-          <t>BANBAJIO CTA: 90201</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="n"/>
-      <c r="E3" s="4" t="n"/>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>BANORTE 9426</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="n"/>
+      <c r="E3" s="5" t="n"/>
       <c r="F3" s="1" t="n"/>
       <c r="G3" s="1" t="n"/>
       <c r="H3" s="1" t="n"/>
@@ -778,42 +714,42 @@
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
       <c r="J5" s="1" t="n"/>
-      <c r="K5" s="59" t="n"/>
-      <c r="L5" s="59" t="n"/>
+      <c r="K5" s="9" t="n"/>
+      <c r="L5" s="9" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="56" t="inlineStr">
-        <is>
-          <t>SALDO EN CONTABILIDAD AL 28 DE FEBRERO 2025</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="n"/>
-      <c r="D6" s="9" t="n"/>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>SALDO EN CONTABILIDAD AL 30 DE JUNIO DEL 2025</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="n"/>
+      <c r="D6" s="11" t="n"/>
       <c r="E6" s="2" t="n"/>
       <c r="F6" s="1" t="n"/>
       <c r="G6" s="1" t="n"/>
-      <c r="H6" s="60" t="n">
-        <v>75372.25</v>
+      <c r="H6" s="12" t="n">
+        <v>549668.6800000001</v>
       </c>
       <c r="I6" s="1" t="n"/>
-      <c r="J6" s="61" t="n"/>
-      <c r="K6" s="59" t="n"/>
-      <c r="L6" s="59" t="n"/>
+      <c r="J6" s="13" t="n"/>
+      <c r="K6" s="9" t="n"/>
+      <c r="L6" s="9" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="n"/>
-      <c r="C7" s="12" t="n"/>
-      <c r="D7" s="12" t="n"/>
+      <c r="C7" s="14" t="n"/>
+      <c r="D7" s="14" t="n"/>
       <c r="E7" s="1" t="n"/>
       <c r="F7" s="1" t="n"/>
       <c r="G7" s="1" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
-      <c r="J7" s="61" t="n"/>
-      <c r="K7" s="59" t="n"/>
-      <c r="L7" s="59" t="n"/>
+      <c r="J7" s="13" t="n"/>
+      <c r="K7" s="9" t="n"/>
+      <c r="L7" s="9" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -826,274 +762,293 @@
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
       <c r="J8" s="1" t="n"/>
-      <c r="K8" s="59" t="n"/>
-      <c r="L8" s="59" t="n"/>
+      <c r="K8" s="9" t="n"/>
+      <c r="L8" s="9" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="57" t="inlineStr">
+      <c r="B9" s="15" t="inlineStr">
         <is>
           <t>DEPOSITOS (+)</t>
         </is>
       </c>
-      <c r="C9" s="13" t="n"/>
-      <c r="D9" s="13" t="n"/>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="14" t="n"/>
-      <c r="G9" s="62" t="n"/>
-      <c r="H9" s="63" t="n">
-        <v>0</v>
+      <c r="C9" s="16" t="n"/>
+      <c r="D9" s="16" t="n"/>
+      <c r="E9" s="5" t="n"/>
+      <c r="F9" s="17" t="n"/>
+      <c r="G9" s="18" t="n"/>
+      <c r="H9" s="19">
+        <f>SUM(A10:G15)</f>
+        <v/>
       </c>
       <c r="I9" s="1" t="n"/>
       <c r="J9" s="1" t="n"/>
-      <c r="K9" s="59" t="n"/>
-      <c r="L9" s="59" t="n"/>
+      <c r="K9" s="9" t="n"/>
+      <c r="L9" s="9" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="64" t="n"/>
-      <c r="B10" s="65" t="n"/>
-      <c r="C10" s="64" t="n"/>
-      <c r="D10" s="65" t="n"/>
-      <c r="E10" s="64" t="n"/>
-      <c r="F10" s="66" t="n"/>
-      <c r="G10" s="67" t="n"/>
-      <c r="H10" s="68" t="n"/>
+      <c r="A10" s="36" t="n">
+        <v>876</v>
+      </c>
+      <c r="B10" s="21" t="n"/>
+      <c r="C10" s="20" t="n"/>
+      <c r="D10" s="21" t="n"/>
+      <c r="E10" s="20" t="n"/>
+      <c r="F10" s="21" t="n"/>
+      <c r="G10" s="20" t="n"/>
+      <c r="H10" s="23" t="n"/>
       <c r="I10" s="1" t="n"/>
       <c r="J10" s="1" t="n"/>
-      <c r="K10" s="59" t="n"/>
-      <c r="L10" s="4" t="n"/>
+      <c r="K10" s="9" t="n"/>
+      <c r="L10" s="5" t="n"/>
       <c r="M10" s="1" t="n"/>
       <c r="N10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="69" t="n"/>
-      <c r="B11" s="70" t="n"/>
-      <c r="C11" s="71" t="n"/>
-      <c r="D11" s="65" t="n"/>
-      <c r="E11" s="64" t="n"/>
-      <c r="F11" s="66" t="n"/>
-      <c r="G11" s="72" t="n"/>
+      <c r="A11" s="36" t="n">
+        <v>6509</v>
+      </c>
+      <c r="B11" s="21" t="n"/>
+      <c r="C11" s="20" t="n"/>
+      <c r="D11" s="21" t="n"/>
+      <c r="E11" s="20" t="n"/>
+      <c r="F11" s="21" t="n"/>
+      <c r="G11" s="20" t="n"/>
       <c r="I11" s="1" t="n"/>
       <c r="J11" s="1" t="n"/>
-      <c r="K11" s="59" t="n"/>
+      <c r="K11" s="9" t="n"/>
       <c r="L11" s="2" t="n"/>
       <c r="M11" s="1" t="n"/>
       <c r="N11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="73" t="n"/>
-      <c r="B12" s="65" t="n"/>
-      <c r="C12" s="74" t="n"/>
-      <c r="D12" s="74" t="n"/>
-      <c r="E12" s="64" t="n"/>
-      <c r="F12" s="66" t="n"/>
-      <c r="G12" s="72" t="n"/>
+      <c r="A12" s="36" t="n">
+        <v>6825.5</v>
+      </c>
+      <c r="B12" s="21" t="n"/>
+      <c r="C12" s="20" t="n"/>
+      <c r="D12" s="21" t="n"/>
+      <c r="E12" s="20" t="n"/>
+      <c r="F12" s="21" t="n"/>
+      <c r="G12" s="20" t="n"/>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
-      <c r="K12" s="59" t="n"/>
-      <c r="L12" s="59" t="n"/>
+      <c r="K12" s="9" t="n"/>
+      <c r="L12" s="9" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="73" t="n"/>
-      <c r="B13" s="65" t="n"/>
-      <c r="C13" s="75" t="n"/>
-      <c r="D13" s="76" t="n"/>
-      <c r="E13" s="64" t="n"/>
-      <c r="F13" s="66" t="n"/>
-      <c r="G13" s="72" t="n"/>
+      <c r="A13" s="36" t="n">
+        <v>9669.5</v>
+      </c>
+      <c r="B13" s="21" t="n"/>
+      <c r="C13" s="20" t="n"/>
+      <c r="D13" s="21" t="n"/>
+      <c r="E13" s="20" t="n"/>
+      <c r="F13" s="21" t="n"/>
+      <c r="G13" s="20" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
       <c r="J13" s="1" t="n"/>
-      <c r="K13" s="59" t="n"/>
-      <c r="L13" s="59" t="n"/>
+      <c r="K13" s="9" t="n"/>
+      <c r="L13" s="9" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="71" t="n"/>
-      <c r="B14" s="70" t="n"/>
-      <c r="C14" s="71" t="n"/>
-      <c r="D14" s="77" t="n"/>
-      <c r="E14" s="64" t="n"/>
-      <c r="F14" s="66" t="n"/>
-      <c r="G14" s="72" t="n"/>
+      <c r="A14" s="36" t="n">
+        <v>10313.5</v>
+      </c>
+      <c r="B14" s="21" t="n"/>
+      <c r="C14" s="20" t="n"/>
+      <c r="D14" s="21" t="n"/>
+      <c r="E14" s="20" t="n"/>
+      <c r="F14" s="21" t="n"/>
+      <c r="G14" s="20" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
       <c r="J14" s="1" t="n"/>
-      <c r="K14" s="59" t="n"/>
-      <c r="L14" s="59" t="n"/>
+      <c r="K14" s="9" t="n"/>
+      <c r="L14" s="9" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="78" t="n"/>
-      <c r="B15" s="74" t="n"/>
-      <c r="C15" s="78" t="n"/>
-      <c r="D15" s="66" t="n"/>
-      <c r="E15" s="73" t="n"/>
-      <c r="F15" s="66" t="n"/>
-      <c r="G15" s="72" t="n"/>
+      <c r="A15" s="36" t="n">
+        <v>21630</v>
+      </c>
+      <c r="B15" s="21" t="n"/>
+      <c r="C15" s="20" t="n"/>
+      <c r="D15" s="21" t="n"/>
+      <c r="E15" s="20" t="n"/>
+      <c r="F15" s="21" t="n"/>
+      <c r="G15" s="20" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
       <c r="J15" s="1" t="n"/>
-      <c r="K15" s="59" t="n"/>
-      <c r="L15" s="59" t="n"/>
+      <c r="K15" s="9" t="n"/>
+      <c r="L15" s="9" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="65" t="n"/>
-      <c r="B16" s="38" t="n"/>
-      <c r="C16" s="65" t="n"/>
-      <c r="D16" s="65" t="n"/>
-      <c r="E16" s="65" t="n"/>
+      <c r="A16" s="21" t="n"/>
+      <c r="B16" s="24" t="n"/>
+      <c r="C16" s="21" t="n"/>
+      <c r="D16" s="21" t="n"/>
+      <c r="E16" s="21" t="n"/>
       <c r="F16" s="2" t="n"/>
-      <c r="G16" s="59" t="n"/>
+      <c r="G16" s="9" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
-      <c r="K16" s="59" t="n"/>
-      <c r="L16" s="59" t="n"/>
+      <c r="K16" s="9" t="n"/>
+      <c r="L16" s="9" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="65" t="n"/>
-      <c r="B17" s="58" t="inlineStr">
+      <c r="A17" s="21" t="n"/>
+      <c r="B17" s="25" t="inlineStr">
         <is>
           <t>RETIROS (-)</t>
         </is>
       </c>
-      <c r="C17" s="65" t="n"/>
-      <c r="D17" s="65" t="n"/>
-      <c r="E17" s="66" t="n"/>
+      <c r="C17" s="21" t="n"/>
+      <c r="D17" s="21" t="n"/>
+      <c r="E17" s="22" t="n"/>
       <c r="F17" s="2" t="n"/>
-      <c r="G17" s="59" t="n"/>
-      <c r="H17" s="79" t="n">
-        <v>0</v>
+      <c r="G17" s="9" t="n"/>
+      <c r="H17" s="26">
+        <f>SUM(A18:G23)</f>
+        <v/>
       </c>
       <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
-      <c r="K17" s="59" t="n"/>
-      <c r="L17" s="59" t="n"/>
+      <c r="K17" s="9" t="n"/>
+      <c r="L17" s="9" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="64" t="n"/>
-      <c r="B18" s="65" t="n"/>
-      <c r="C18" s="64" t="n"/>
-      <c r="D18" s="65" t="n"/>
-      <c r="E18" s="64" t="n"/>
-      <c r="F18" s="66" t="n"/>
-      <c r="G18" s="67" t="n"/>
+      <c r="A18" s="36" t="n">
+        <v>827</v>
+      </c>
+      <c r="B18" s="21" t="n"/>
+      <c r="C18" s="20" t="n"/>
+      <c r="D18" s="21" t="n"/>
+      <c r="E18" s="20" t="n"/>
+      <c r="F18" s="21" t="n"/>
+      <c r="G18" s="20" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
       <c r="J18" s="1" t="n"/>
-      <c r="K18" s="59" t="n"/>
-      <c r="L18" s="59" t="n"/>
+      <c r="K18" s="9" t="n"/>
+      <c r="L18" s="9" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="69" t="n"/>
-      <c r="B19" s="70" t="n"/>
-      <c r="C19" s="71" t="n"/>
-      <c r="D19" s="65" t="n"/>
-      <c r="E19" s="64" t="n"/>
-      <c r="F19" s="66" t="n"/>
-      <c r="G19" s="72" t="n"/>
+      <c r="A19" s="36" t="n">
+        <v>2291.71</v>
+      </c>
+      <c r="B19" s="21" t="n"/>
+      <c r="C19" s="20" t="n"/>
+      <c r="D19" s="21" t="n"/>
+      <c r="E19" s="20" t="n"/>
+      <c r="F19" s="21" t="n"/>
+      <c r="G19" s="20" t="n"/>
       <c r="H19" s="1" t="n"/>
       <c r="I19" s="1" t="n"/>
       <c r="J19" s="1" t="n"/>
-      <c r="K19" s="59" t="n"/>
-      <c r="L19" s="59" t="n"/>
+      <c r="K19" s="9" t="n"/>
+      <c r="L19" s="9" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="73" t="n"/>
-      <c r="B20" s="65" t="n"/>
-      <c r="C20" s="74" t="n"/>
-      <c r="D20" s="74" t="n"/>
-      <c r="E20" s="64" t="n"/>
-      <c r="F20" s="66" t="n"/>
-      <c r="G20" s="72" t="n"/>
+      <c r="A20" s="20" t="n"/>
+      <c r="B20" s="21" t="n"/>
+      <c r="C20" s="20" t="n"/>
+      <c r="D20" s="21" t="n"/>
+      <c r="E20" s="20" t="n"/>
+      <c r="F20" s="21" t="n"/>
+      <c r="G20" s="20" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
       <c r="J20" s="1" t="n"/>
-      <c r="K20" s="59" t="n"/>
-      <c r="L20" s="59" t="n"/>
+      <c r="K20" s="9" t="n"/>
+      <c r="L20" s="9" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="73" t="n"/>
-      <c r="B21" s="65" t="n"/>
-      <c r="C21" s="75" t="n"/>
-      <c r="D21" s="76" t="n"/>
-      <c r="E21" s="64" t="n"/>
-      <c r="F21" s="66" t="n"/>
-      <c r="G21" s="72" t="n"/>
+      <c r="A21" s="20" t="n"/>
+      <c r="B21" s="21" t="n"/>
+      <c r="C21" s="20" t="n"/>
+      <c r="D21" s="21" t="n"/>
+      <c r="E21" s="20" t="n"/>
+      <c r="F21" s="21" t="n"/>
+      <c r="G21" s="20" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
       <c r="J21" s="1" t="n"/>
-      <c r="K21" s="59" t="n"/>
-      <c r="L21" s="59" t="n"/>
+      <c r="K21" s="9" t="n"/>
+      <c r="L21" s="9" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="71" t="n"/>
-      <c r="B22" s="70" t="n"/>
-      <c r="C22" s="71" t="n"/>
-      <c r="D22" s="77" t="n"/>
-      <c r="E22" s="64" t="n"/>
-      <c r="F22" s="66" t="n"/>
-      <c r="G22" s="72" t="n"/>
+      <c r="A22" s="20" t="n"/>
+      <c r="B22" s="21" t="n"/>
+      <c r="C22" s="20" t="n"/>
+      <c r="D22" s="21" t="n"/>
+      <c r="E22" s="20" t="n"/>
+      <c r="F22" s="21" t="n"/>
+      <c r="G22" s="20" t="n"/>
       <c r="I22" s="1" t="n"/>
       <c r="J22" s="1" t="n"/>
-      <c r="K22" s="59" t="n"/>
-      <c r="L22" s="59" t="n"/>
+      <c r="K22" s="9" t="n"/>
+      <c r="L22" s="9" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="78" t="n"/>
-      <c r="B23" s="74" t="n"/>
-      <c r="C23" s="78" t="n"/>
-      <c r="D23" s="66" t="n"/>
-      <c r="E23" s="73" t="n"/>
-      <c r="F23" s="66" t="n"/>
-      <c r="G23" s="72" t="n"/>
-      <c r="H23" s="80" t="n"/>
+      <c r="A23" s="20" t="n"/>
+      <c r="B23" s="21" t="n"/>
+      <c r="C23" s="20" t="n"/>
+      <c r="D23" s="21" t="n"/>
+      <c r="E23" s="20" t="n"/>
+      <c r="F23" s="21" t="n"/>
+      <c r="G23" s="20" t="n"/>
+      <c r="H23" s="27" t="n"/>
       <c r="I23" s="1" t="n"/>
-      <c r="J23" s="61" t="n"/>
-      <c r="K23" s="59" t="n"/>
-      <c r="L23" s="59" t="n"/>
+      <c r="J23" s="13" t="n"/>
+      <c r="K23" s="9" t="n"/>
+      <c r="L23" s="9" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="65" t="n"/>
-      <c r="B24" s="65" t="n"/>
-      <c r="C24" s="65" t="n"/>
-      <c r="D24" s="66" t="n"/>
+      <c r="A24" s="21" t="n"/>
+      <c r="B24" s="21" t="n"/>
+      <c r="C24" s="21" t="n"/>
+      <c r="D24" s="22" t="n"/>
       <c r="E24" s="1" t="n"/>
       <c r="F24" s="2" t="n"/>
       <c r="G24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
-      <c r="J24" s="61" t="n"/>
-      <c r="K24" s="59" t="n"/>
-      <c r="L24" s="59" t="n"/>
+      <c r="J24" s="13" t="n"/>
+      <c r="K24" s="9" t="n"/>
+      <c r="L24" s="9" t="n"/>
     </row>
     <row r="25">
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>DIFERENCIA</t>
+          <t>SALDO EN LIBROS</t>
         </is>
       </c>
       <c r="G25" s="2" t="n"/>
-      <c r="H25" s="60" t="n">
-        <v>75372.25</v>
+      <c r="H25" s="12">
+        <f>+H6+H9-H17</f>
+        <v/>
       </c>
       <c r="I25" s="1" t="n"/>
       <c r="J25" s="1" t="n"/>
-      <c r="K25" s="59" t="n"/>
-      <c r="L25" s="59" t="n"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="81" t="n"/>
-      <c r="B26" s="81" t="n"/>
-      <c r="C26" s="81" t="n"/>
-      <c r="D26" s="81" t="n"/>
-      <c r="E26" s="45" t="n"/>
-      <c r="F26" s="45" t="n"/>
-      <c r="G26" s="45" t="n"/>
-      <c r="H26" s="45" t="n"/>
+      <c r="K25" s="9" t="n"/>
+      <c r="L25" s="9" t="n"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="28" t="n"/>
+      <c r="B26" s="28" t="n"/>
+      <c r="C26" s="28" t="n"/>
+      <c r="D26" s="28" t="n"/>
+      <c r="E26" s="29" t="n"/>
+      <c r="F26" s="29" t="n"/>
+      <c r="G26" s="29" t="n"/>
+      <c r="H26" s="29" t="n"/>
       <c r="I26" s="1" t="n"/>
-      <c r="J26" s="61" t="n"/>
-      <c r="K26" s="59" t="n"/>
-      <c r="L26" s="59" t="n"/>
+      <c r="J26" s="13" t="n"/>
+      <c r="K26" s="9" t="n"/>
+      <c r="L26" s="9" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
@@ -1104,10 +1059,10 @@
       <c r="F27" s="1" t="n"/>
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
-      <c r="I27" s="82" t="n"/>
-      <c r="J27" s="61" t="n"/>
-      <c r="K27" s="59" t="n"/>
-      <c r="L27" s="59" t="n"/>
+      <c r="I27" s="30" t="n"/>
+      <c r="J27" s="13" t="n"/>
+      <c r="K27" s="9" t="n"/>
+      <c r="L27" s="9" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
@@ -1117,16 +1072,16 @@
         </is>
       </c>
       <c r="C28" s="2" t="n"/>
-      <c r="E28" s="47" t="n"/>
-      <c r="F28" s="83" t="n"/>
-      <c r="G28" s="65" t="n"/>
-      <c r="H28" s="60" t="n">
-        <v>76728.27</v>
+      <c r="E28" s="31" t="n"/>
+      <c r="F28" s="32" t="n"/>
+      <c r="G28" s="21" t="n"/>
+      <c r="H28" s="12" t="n">
+        <v>549706.17</v>
       </c>
       <c r="I28" s="1" t="n"/>
-      <c r="J28" s="61" t="n"/>
-      <c r="K28" s="59" t="n"/>
-      <c r="L28" s="59" t="n"/>
+      <c r="J28" s="13" t="n"/>
+      <c r="K28" s="9" t="n"/>
+      <c r="L28" s="9" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
@@ -1143,8 +1098,8 @@
       </c>
       <c r="I29" s="1" t="n"/>
       <c r="J29" s="1" t="n"/>
-      <c r="K29" s="59" t="n"/>
-      <c r="L29" s="59" t="n"/>
+      <c r="K29" s="9" t="n"/>
+      <c r="L29" s="9" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
@@ -1157,198 +1112,212 @@
       <c r="H30" s="1" t="n"/>
       <c r="I30" s="1" t="n"/>
       <c r="J30" s="1" t="n"/>
-      <c r="K30" s="59" t="n"/>
-      <c r="L30" s="59" t="n"/>
+      <c r="K30" s="9" t="n"/>
+      <c r="L30" s="9" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="B31" s="5" t="inlineStr">
         <is>
           <t>DEPOSITOS EN TRANSITO (+)</t>
         </is>
       </c>
-      <c r="C31" s="4" t="n"/>
-      <c r="D31" s="4" t="n"/>
+      <c r="C31" s="5" t="n"/>
+      <c r="D31" s="5" t="n"/>
       <c r="E31" s="1" t="n"/>
       <c r="F31" s="1" t="n"/>
       <c r="G31" s="1" t="n"/>
-      <c r="H31" s="63" t="n">
-        <v>0</v>
+      <c r="H31" s="19">
+        <f>SUM(A32:G37)</f>
+        <v/>
       </c>
       <c r="I31" s="1" t="n"/>
       <c r="J31" s="1" t="n"/>
-      <c r="K31" s="59" t="n"/>
-      <c r="L31" s="59" t="n"/>
+      <c r="K31" s="9" t="n"/>
+      <c r="L31" s="9" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="64" t="n"/>
-      <c r="B32" s="65" t="n"/>
-      <c r="C32" s="64" t="n"/>
-      <c r="D32" s="65" t="n"/>
-      <c r="E32" s="64" t="n"/>
-      <c r="F32" s="66" t="n"/>
-      <c r="G32" s="67" t="n"/>
+      <c r="A32" s="36" t="n">
+        <v>827</v>
+      </c>
+      <c r="B32" s="21" t="n"/>
+      <c r="C32" s="20" t="n"/>
+      <c r="D32" s="21" t="n"/>
+      <c r="E32" s="20" t="n"/>
+      <c r="F32" s="21" t="n"/>
+      <c r="G32" s="20" t="n"/>
       <c r="H32" s="1" t="n"/>
       <c r="I32" s="1" t="n"/>
       <c r="J32" s="1" t="n"/>
-      <c r="K32" s="59" t="n"/>
-      <c r="L32" s="59" t="n"/>
+      <c r="K32" s="9" t="n"/>
+      <c r="L32" s="9" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="69" t="n"/>
-      <c r="B33" s="70" t="n"/>
-      <c r="C33" s="71" t="n"/>
-      <c r="D33" s="65" t="n"/>
-      <c r="E33" s="64" t="n"/>
-      <c r="F33" s="66" t="n"/>
-      <c r="G33" s="72" t="n"/>
+      <c r="A33" s="36" t="n">
+        <v>884</v>
+      </c>
+      <c r="B33" s="21" t="n"/>
+      <c r="C33" s="20" t="n"/>
+      <c r="D33" s="21" t="n"/>
+      <c r="E33" s="20" t="n"/>
+      <c r="F33" s="21" t="n"/>
+      <c r="G33" s="20" t="n"/>
       <c r="H33" s="1" t="n"/>
       <c r="I33" s="1" t="n"/>
       <c r="J33" s="1" t="n"/>
-      <c r="K33" s="59" t="n"/>
-      <c r="L33" s="59" t="n"/>
+      <c r="K33" s="9" t="n"/>
+      <c r="L33" s="9" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="73" t="n"/>
-      <c r="B34" s="65" t="n"/>
-      <c r="C34" s="74" t="n"/>
-      <c r="D34" s="74" t="n"/>
-      <c r="E34" s="64" t="n"/>
-      <c r="F34" s="66" t="n"/>
-      <c r="G34" s="72" t="n"/>
+      <c r="A34" s="36" t="n">
+        <v>9699.5</v>
+      </c>
+      <c r="B34" s="21" t="n"/>
+      <c r="C34" s="20" t="n"/>
+      <c r="D34" s="21" t="n"/>
+      <c r="E34" s="20" t="n"/>
+      <c r="F34" s="21" t="n"/>
+      <c r="G34" s="20" t="n"/>
       <c r="H34" s="1" t="n"/>
       <c r="I34" s="1" t="n"/>
       <c r="J34" s="1" t="n"/>
-      <c r="K34" s="66" t="n"/>
+      <c r="K34" s="22" t="n"/>
       <c r="L34" s="1" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="73" t="n"/>
-      <c r="B35" s="65" t="n"/>
-      <c r="C35" s="75" t="n"/>
-      <c r="D35" s="76" t="n"/>
-      <c r="E35" s="64" t="n"/>
-      <c r="F35" s="66" t="n"/>
-      <c r="G35" s="72" t="n"/>
+      <c r="A35" s="36" t="n">
+        <v>17139</v>
+      </c>
+      <c r="B35" s="21" t="n"/>
+      <c r="C35" s="20" t="n"/>
+      <c r="D35" s="21" t="n"/>
+      <c r="E35" s="20" t="n"/>
+      <c r="F35" s="21" t="n"/>
+      <c r="G35" s="20" t="n"/>
       <c r="H35" s="1" t="n"/>
       <c r="I35" s="1" t="n"/>
       <c r="J35" s="1" t="n"/>
-      <c r="K35" s="65" t="n"/>
+      <c r="K35" s="21" t="n"/>
       <c r="L35" s="1" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="71" t="n"/>
-      <c r="B36" s="70" t="n"/>
-      <c r="C36" s="71" t="n"/>
-      <c r="D36" s="77" t="n"/>
-      <c r="E36" s="64" t="n"/>
-      <c r="F36" s="66" t="n"/>
-      <c r="G36" s="72" t="n"/>
+      <c r="A36" s="36" t="n">
+        <v>21629.5</v>
+      </c>
+      <c r="B36" s="21" t="n"/>
+      <c r="C36" s="20" t="n"/>
+      <c r="D36" s="21" t="n"/>
+      <c r="E36" s="20" t="n"/>
+      <c r="F36" s="21" t="n"/>
+      <c r="G36" s="20" t="n"/>
       <c r="I36" s="1" t="n"/>
       <c r="J36" s="1" t="n"/>
-      <c r="K36" s="66" t="n"/>
+      <c r="K36" s="22" t="n"/>
       <c r="L36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="78" t="n"/>
-      <c r="B37" s="74" t="n"/>
-      <c r="C37" s="78" t="n"/>
-      <c r="D37" s="66" t="n"/>
-      <c r="E37" s="73" t="n"/>
-      <c r="F37" s="66" t="n"/>
-      <c r="G37" s="72" t="n"/>
-      <c r="H37" s="59" t="n"/>
+      <c r="A37" s="36" t="n">
+        <v>550248.47</v>
+      </c>
+      <c r="B37" s="21" t="n"/>
+      <c r="C37" s="20" t="n"/>
+      <c r="D37" s="21" t="n"/>
+      <c r="E37" s="20" t="n"/>
+      <c r="F37" s="21" t="n"/>
+      <c r="G37" s="20" t="n"/>
+      <c r="H37" s="9" t="n"/>
       <c r="I37" s="1" t="n"/>
       <c r="J37" s="1" t="n"/>
-      <c r="K37" s="66" t="n"/>
+      <c r="K37" s="22" t="n"/>
       <c r="L37" s="1" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="59" t="n"/>
-      <c r="B38" s="59" t="n"/>
+      <c r="A38" s="9" t="n"/>
+      <c r="B38" s="9" t="n"/>
       <c r="C38" s="1" t="n"/>
       <c r="D38" s="1" t="n"/>
       <c r="E38" s="2" t="n"/>
       <c r="F38" s="1" t="n"/>
-      <c r="G38" s="59" t="n"/>
+      <c r="G38" s="9" t="n"/>
       <c r="H38" s="1" t="n"/>
       <c r="I38" s="1" t="n"/>
       <c r="J38" s="1" t="n"/>
-      <c r="K38" s="66" t="n"/>
+      <c r="K38" s="22" t="n"/>
       <c r="L38" s="1" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="59" t="n"/>
-      <c r="B39" s="58" t="inlineStr">
+      <c r="A39" s="9" t="n"/>
+      <c r="B39" s="25" t="inlineStr">
         <is>
           <t>CHEQUES EN TRANSITO (-)</t>
         </is>
       </c>
-      <c r="C39" s="84" t="n"/>
-      <c r="D39" s="84" t="n"/>
+      <c r="C39" s="33" t="n"/>
+      <c r="D39" s="33" t="n"/>
       <c r="E39" s="2" t="n"/>
       <c r="F39" s="1" t="n"/>
-      <c r="G39" s="59" t="n"/>
-      <c r="H39" s="79" t="n">
-        <v>1356.81</v>
+      <c r="G39" s="9" t="n"/>
+      <c r="H39" s="26">
+        <f>SUM(A40:G45)</f>
+        <v/>
       </c>
       <c r="I39" s="1" t="n"/>
       <c r="J39" s="1" t="n"/>
-      <c r="K39" s="66" t="n"/>
+      <c r="K39" s="22" t="n"/>
       <c r="L39" s="1" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="64" t="n">
-        <v>1356.81</v>
-      </c>
-      <c r="B40" s="65" t="n"/>
-      <c r="C40" s="64" t="n"/>
-      <c r="D40" s="65" t="n"/>
-      <c r="E40" s="64" t="n"/>
-      <c r="F40" s="66" t="n"/>
-      <c r="G40" s="67" t="n"/>
+      <c r="A40" s="36" t="n">
+        <v>2291.72</v>
+      </c>
+      <c r="B40" s="21" t="n"/>
+      <c r="C40" s="20" t="n"/>
+      <c r="D40" s="21" t="n"/>
+      <c r="E40" s="20" t="n"/>
+      <c r="F40" s="21" t="n"/>
+      <c r="G40" s="20" t="n"/>
       <c r="I40" s="1" t="n"/>
       <c r="J40" s="1" t="n"/>
-      <c r="K40" s="66" t="n"/>
+      <c r="K40" s="22" t="n"/>
       <c r="L40" s="1" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="69" t="n"/>
-      <c r="B41" s="70" t="n"/>
-      <c r="C41" s="71" t="n"/>
-      <c r="D41" s="65" t="n"/>
-      <c r="E41" s="64" t="n"/>
-      <c r="F41" s="66" t="n"/>
-      <c r="G41" s="72" t="n"/>
+      <c r="A41" s="20" t="n"/>
+      <c r="B41" s="21" t="n"/>
+      <c r="C41" s="20" t="n"/>
+      <c r="D41" s="21" t="n"/>
+      <c r="E41" s="20" t="n"/>
+      <c r="F41" s="21" t="n"/>
+      <c r="G41" s="20" t="n"/>
       <c r="H41" s="1" t="n"/>
       <c r="I41" s="1" t="n"/>
       <c r="J41" s="1" t="n"/>
-      <c r="K41" s="66" t="n"/>
+      <c r="K41" s="22" t="n"/>
       <c r="L41" s="1" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="73" t="n"/>
-      <c r="B42" s="65" t="n"/>
-      <c r="C42" s="74" t="n"/>
-      <c r="D42" s="74" t="n"/>
-      <c r="E42" s="64" t="n"/>
-      <c r="F42" s="66" t="n"/>
-      <c r="G42" s="72" t="n"/>
+      <c r="A42" s="20" t="n"/>
+      <c r="B42" s="21" t="n"/>
+      <c r="C42" s="20" t="n"/>
+      <c r="D42" s="21" t="n"/>
+      <c r="E42" s="20" t="n"/>
+      <c r="F42" s="21" t="n"/>
+      <c r="G42" s="20" t="n"/>
       <c r="H42" s="1" t="n"/>
       <c r="I42" s="1" t="n"/>
       <c r="J42" s="1" t="n"/>
-      <c r="K42" s="66" t="n"/>
+      <c r="K42" s="22" t="n"/>
       <c r="L42" s="1" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="73" t="n"/>
-      <c r="B43" s="65" t="n"/>
-      <c r="C43" s="75" t="n"/>
-      <c r="D43" s="76" t="n"/>
-      <c r="E43" s="64" t="n"/>
-      <c r="F43" s="66" t="n"/>
-      <c r="G43" s="72" t="n"/>
-      <c r="H43" s="62" t="inlineStr">
+      <c r="A43" s="20" t="n"/>
+      <c r="B43" s="21" t="n"/>
+      <c r="C43" s="20" t="n"/>
+      <c r="D43" s="21" t="n"/>
+      <c r="E43" s="20" t="n"/>
+      <c r="F43" s="21" t="n"/>
+      <c r="G43" s="20" t="n"/>
+      <c r="H43" s="18" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -1359,13 +1328,13 @@
       <c r="L43" s="1" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="71" t="n"/>
-      <c r="B44" s="70" t="n"/>
-      <c r="C44" s="71" t="n"/>
-      <c r="D44" s="77" t="n"/>
-      <c r="E44" s="64" t="n"/>
-      <c r="F44" s="66" t="n"/>
-      <c r="G44" s="72" t="n"/>
+      <c r="A44" s="20" t="n"/>
+      <c r="B44" s="21" t="n"/>
+      <c r="C44" s="20" t="n"/>
+      <c r="D44" s="21" t="n"/>
+      <c r="E44" s="20" t="n"/>
+      <c r="F44" s="21" t="n"/>
+      <c r="G44" s="20" t="n"/>
       <c r="H44" s="1" t="n"/>
       <c r="I44" s="1" t="n"/>
       <c r="J44" s="1" t="n"/>
@@ -1373,25 +1342,25 @@
       <c r="L44" s="1" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="78" t="n"/>
-      <c r="B45" s="74" t="n"/>
-      <c r="C45" s="78" t="n"/>
-      <c r="D45" s="66" t="n"/>
-      <c r="E45" s="73" t="n"/>
-      <c r="F45" s="66" t="n"/>
-      <c r="G45" s="72" t="n"/>
+      <c r="A45" s="20" t="n"/>
+      <c r="B45" s="21" t="n"/>
+      <c r="C45" s="20" t="n"/>
+      <c r="D45" s="21" t="n"/>
+      <c r="E45" s="20" t="n"/>
+      <c r="F45" s="21" t="n"/>
+      <c r="G45" s="20" t="n"/>
       <c r="I45" s="1" t="n"/>
       <c r="J45" s="1" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="62" t="n"/>
-      <c r="B46" s="62" t="n"/>
-      <c r="C46" s="62" t="n"/>
-      <c r="D46" s="62" t="n"/>
+      <c r="A46" s="18" t="n"/>
+      <c r="B46" s="18" t="n"/>
+      <c r="C46" s="18" t="n"/>
+      <c r="D46" s="18" t="n"/>
       <c r="I46" s="1" t="n"/>
       <c r="J46" s="1" t="n"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1" thickBot="1">
+    <row r="47">
       <c r="E47" s="2" t="inlineStr">
         <is>
           <t>SALDO EN BANCOS</t>
@@ -1399,15 +1368,16 @@
       </c>
       <c r="F47" s="1" t="n"/>
       <c r="G47" s="1" t="n"/>
-      <c r="H47" s="85" t="n">
-        <v>75371.46000000001</v>
+      <c r="H47" s="34">
+        <f>SUM(H28+H31-H39)</f>
+        <v/>
       </c>
       <c r="I47" s="1" t="n"/>
       <c r="J47" s="1" t="n"/>
       <c r="K47" s="1" t="n"/>
       <c r="L47" s="1" t="n"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1" thickTop="1">
+    <row r="48">
       <c r="E48" s="2" t="inlineStr">
         <is>
           <t>SOBRANTE</t>
@@ -1415,8 +1385,9 @@
       </c>
       <c r="F48" s="1" t="n"/>
       <c r="G48" s="1" t="n"/>
-      <c r="H48" s="86" t="n">
-        <v>0.7899999999935972</v>
+      <c r="H48" s="35">
+        <f>+H47-H25</f>
+        <v/>
       </c>
       <c r="I48" s="1" t="n"/>
       <c r="J48" s="1" t="n"/>
@@ -1428,7 +1399,7 @@
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.7480314960629921" bottom="0.7480314960629921" header="0.3149606299212598" footer="0.3149606299212598"/>
-  <pageSetup orientation="portrait" scale="74"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" scale="74" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>